<commit_message>
edited biospecimen collection protocol and timeline as per Victoria's corrections
</commit_message>
<xml_diff>
--- a/inst/extdata/biospecimen_collection_for_biostore_calculations.xlsx
+++ b/inst/extdata/biospecimen_collection_for_biostore_calculations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanshilts/r_code/biostoreCapacity/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF095A98-4604-E74B-BE05-8A0DA41BB87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23599AE5-0BD1-574D-AB66-2E1ACA35384A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="2900" windowWidth="30780" windowHeight="17380" xr2:uid="{F08E2CC1-CD3C-F641-B418-A953A5DB15A9}"/>
+    <workbookView xWindow="10760" yWindow="2820" windowWidth="23960" windowHeight="17380" xr2:uid="{F08E2CC1-CD3C-F641-B418-A953A5DB15A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="63">
   <si>
     <t>whole_blood_maternal</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>collection_id</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>this was removed for 2025, but Victoria not sure about beyond that</t>
+  </si>
+  <si>
+    <t>set to 1 because this wasn't officially changed. We couldn't remove this collection until we added 11-17 blood spot (which needed IRB approval) so i think it was decided this would change in 2026 to add 11-17 blood spot and remove 11-17 whole blood in 2026</t>
+  </si>
+  <si>
+    <t>set to 1 because this wasn't officially changed. We couldn't remove this collection until we added 11-17 blood spot (which needed IRB approval) so i think it was decided this would change in 2026 to add 11-17 blood spot and remove 11-17 whole blood in 202</t>
   </si>
 </sst>
 </file>
@@ -249,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -272,15 +284,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,21 +327,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -344,21 +378,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -377,6 +404,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -390,6 +424,63 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -415,13 +506,8 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -430,58 +516,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -828,10 +862,10 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,10 +887,10 @@
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="29.1640625" customWidth="1"/>
     <col min="27" max="27" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.33203125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
@@ -941,8 +975,11 @@
       <c r="AB1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="AC1" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>B2&amp;"_"&amp;E2&amp;"_"&amp;H2&amp;"_"&amp;J2</f>
         <v>breastmilk_1.9ml_0_5_months_specialized</v>
@@ -1028,8 +1065,11 @@
       <c r="AB2" s="1">
         <v>0.5</v>
       </c>
+      <c r="AC2" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A28" si="0">B3&amp;"_"&amp;E3&amp;"_"&amp;H3&amp;"_"&amp;J3</f>
         <v>breastmilk_1ml_0_5_months_specialized</v>
@@ -1115,8 +1155,11 @@
       <c r="AB3" s="1">
         <v>0.5</v>
       </c>
+      <c r="AC3" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>cord_blood_1.9ml_perinatal_core</v>
@@ -1202,8 +1245,11 @@
       <c r="AB4" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>cord_blood_1ml_perinatal_core</v>
@@ -1289,8 +1335,11 @@
       <c r="AB5" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>placenta_1.9ml_perinatal_core</v>
@@ -1376,8 +1425,11 @@
       <c r="AB6" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC6" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_maternal_1.9ml_preg_early_core</v>
@@ -1463,8 +1515,11 @@
       <c r="AB7" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC7" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_maternal_1.9ml_preg_third_tri_core</v>
@@ -1550,8 +1605,11 @@
       <c r="AB8" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC8" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>urine_diaper_1.9ml_0_5_months_core</v>
@@ -1637,8 +1695,11 @@
       <c r="AB9" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_current_partner_1.9ml_6_11_months_preconception</v>
@@ -1671,7 +1732,7 @@
         <v>41</v>
       </c>
       <c r="K10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
@@ -1724,8 +1785,11 @@
       <c r="AB10" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC10" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_maternal_1.9ml_6_11_months_preconception</v>
@@ -1811,8 +1875,11 @@
       <c r="AB11" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC11" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>urine_diaper_1.9ml_12_23_months_specialized</v>
@@ -1898,8 +1965,11 @@
       <c r="AB12" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC12" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_maternal_1.9ml_24_35_months_preconception</v>
@@ -1932,7 +2002,7 @@
         <v>41</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
@@ -1985,8 +2055,11 @@
       <c r="AB13" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC13" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>urine_hat_1.9ml_3_5_years_core</v>
@@ -2072,8 +2145,11 @@
       <c r="AB14" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC14" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>urine_hat_1.9ml_6_10_years_core</v>
@@ -2159,8 +2235,11 @@
       <c r="AB15" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC15" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>urine_cup_child_1.9ml_11_17_years_core</v>
@@ -2246,8 +2325,11 @@
       <c r="AB16" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC16" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_maternal_1.9ml_preg_early_core</v>
@@ -2333,8 +2415,11 @@
       <c r="AB17" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC17" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_maternal_1.9ml_preg_third_tri_core</v>
@@ -2420,8 +2505,11 @@
       <c r="AB18" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC18" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1.9ml_6_10_years_specialized</v>
@@ -2507,8 +2595,11 @@
       <c r="AB19" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC19" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1.9ml_6_10_years_core</v>
@@ -2594,8 +2685,11 @@
       <c r="AB20" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC20" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1.9ml_11_17_years_specialized</v>
@@ -2681,8 +2775,11 @@
       <c r="AB21" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC21" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1.9ml_11_17_years_core</v>
@@ -2715,7 +2812,7 @@
         <v>22</v>
       </c>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="1">
         <v>0</v>
@@ -2768,8 +2865,11 @@
       <c r="AB22" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC22" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_maternal_1ml_preg_early_core</v>
@@ -2855,8 +2955,11 @@
       <c r="AB23" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC23" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_maternal_1ml_preg_third_tri_core</v>
@@ -2942,8 +3045,11 @@
       <c r="AB24" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC24" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1ml_6_10_years_specialized</v>
@@ -3029,8 +3135,11 @@
       <c r="AB25" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC25" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1ml_6_10_years_core</v>
@@ -3116,8 +3225,11 @@
       <c r="AB26" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC26" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1ml_11_17_years_specialized</v>
@@ -3203,8 +3315,11 @@
       <c r="AB27" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AC27" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>whole_blood_child_1ml_11_17_years_core</v>
@@ -3237,7 +3352,7 @@
         <v>22</v>
       </c>
       <c r="K28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" s="1">
         <v>0</v>
@@ -3289,6 +3404,9 @@
       </c>
       <c r="AB28" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="AC28" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3300,41 +3418,41 @@
     <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="placenta">
       <formula>NOT(ISERROR(SEARCH("placenta",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="urine">
-      <formula>NOT(ISERROR(SEARCH("urine",C1)))</formula>
+    <cfRule type="containsText" dxfId="22" priority="16" operator="containsText" text="whole_blood">
+      <formula>NOT(ISERROR(SEARCH("whole_blood",C1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="cord_blood">
       <formula>NOT(ISERROR(SEARCH("cord_blood",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="whole_blood">
-      <formula>NOT(ISERROR(SEARCH("whole_blood",C1)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="14" operator="containsText" text="urine">
+      <formula>NOT(ISERROR(SEARCH("urine",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576 H7:I8 H15:I24">
-    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="partner">
-      <formula>NOT(ISERROR(SEARCH("partner",D1)))</formula>
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="maternal">
+      <formula>NOT(ISERROR(SEARCH("maternal",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="child">
       <formula>NOT(ISERROR(SEARCH("child",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="maternal">
-      <formula>NOT(ISERROR(SEARCH("maternal",D1)))</formula>
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="partner">
+      <formula>NOT(ISERROR(SEARCH("partner",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="1.9ml">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="1ml">
+      <formula>NOT(ISERROR(SEARCH("1ml",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="1.9ml">
       <formula>NOT(ISERROR(SEARCH("1.9ml",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="1ml">
-      <formula>NOT(ISERROR(SEARCH("1ml",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="11_17_years">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="6_10_years">
+      <formula>NOT(ISERROR(SEARCH("6_10_years",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="11_17_years">
       <formula>NOT(ISERROR(SEARCH("11_17_years",H1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="6_10_years">
-      <formula>NOT(ISERROR(SEARCH("6_10_years",H1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="perinatal">
       <formula>NOT(ISERROR(SEARCH("perinatal",H1)))</formula>
@@ -3344,20 +3462,20 @@
     <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="preg_third_tri">
       <formula>NOT(ISERROR(SEARCH("preg_third_tri",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="preg_early">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="6_11_months">
+      <formula>NOT(ISERROR(SEARCH("6_11_months",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="preg_early">
       <formula>NOT(ISERROR(SEARCH("preg_early",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="24_35_months">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="24_35_months">
       <formula>NOT(ISERROR(SEARCH("24_35_months",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="12_23_months">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="0_5_months">
+      <formula>NOT(ISERROR(SEARCH("0_5_months",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="12_23_months">
       <formula>NOT(ISERROR(SEARCH("12_23_months",H1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="6_11_months">
-      <formula>NOT(ISERROR(SEARCH("6_11_months",H1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="0_5_months">
-      <formula>NOT(ISERROR(SEARCH("0_5_months",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
@@ -3372,14 +3490,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:P1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="11" operator="beginsWith" text="0">
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",K1)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="11" operator="beginsWith" text="0">
       <formula>LEFT(K1,LEN("0"))="0"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="12" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",K1)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W1:AB1048576">
+  <conditionalFormatting sqref="W1:AB1048576 AC10:AC28">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",W1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
added more info to readme and changed column names of input data so they're more intuitive
</commit_message>
<xml_diff>
--- a/inst/extdata/biospecimen_collection_for_biostore_calculations.xlsx
+++ b/inst/extdata/biospecimen_collection_for_biostore_calculations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanshilts/r_code/biostoreCapacity/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23599AE5-0BD1-574D-AB66-2E1ACA35384A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995CADB5-E65F-6943-AF5C-360FC78F0C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2820" windowWidth="23960" windowHeight="17380" xr2:uid="{F08E2CC1-CD3C-F641-B418-A953A5DB15A9}"/>
+    <workbookView xWindow="9400" yWindow="7220" windowWidth="23960" windowHeight="17380" xr2:uid="{F08E2CC1-CD3C-F641-B418-A953A5DB15A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,24 +140,6 @@
     <t>specimen_type</t>
   </si>
   <si>
-    <t>y_2025_multiplier</t>
-  </si>
-  <si>
-    <t>y_2026_multiplier</t>
-  </si>
-  <si>
-    <t>y_2027_multiplier</t>
-  </si>
-  <si>
-    <t>y_2028_multiplier</t>
-  </si>
-  <si>
-    <t>y_2029_multiplier</t>
-  </si>
-  <si>
-    <t>y_2030_multiplier</t>
-  </si>
-  <si>
     <t>6_11_months</t>
   </si>
   <si>
@@ -191,21 +173,12 @@
     <t>NA</t>
   </si>
   <si>
-    <t>specialized_obesity_multiplier</t>
-  </si>
-  <si>
     <t>specialized_chemphys</t>
   </si>
   <si>
-    <t>specialized_chemphys_multiplier</t>
-  </si>
-  <si>
     <t>specialized_lifestyle</t>
   </si>
   <si>
-    <t>specialized_lifestyle_multiplier</t>
-  </si>
-  <si>
     <t>visit_logical_order</t>
   </si>
   <si>
@@ -225,6 +198,33 @@
   </si>
   <si>
     <t>set to 1 because this wasn't officially changed. We couldn't remove this collection until we added 11-17 blood spot (which needed IRB approval) so i think it was decided this would change in 2026 to add 11-17 blood spot and remove 11-17 whole blood in 202</t>
+  </si>
+  <si>
+    <t>y_2025_proportion</t>
+  </si>
+  <si>
+    <t>y_2026_proportion</t>
+  </si>
+  <si>
+    <t>y_2027_proportion</t>
+  </si>
+  <si>
+    <t>y_2028_proportion</t>
+  </si>
+  <si>
+    <t>y_2029_proportion</t>
+  </si>
+  <si>
+    <t>y_2030_proportion</t>
+  </si>
+  <si>
+    <t>specialized_obesity_proportion</t>
+  </si>
+  <si>
+    <t>specialized_chemphys_proportion</t>
+  </si>
+  <si>
+    <t>specialized_lifestyle_proportion</t>
   </si>
 </sst>
 </file>
@@ -313,8 +313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,10 +862,10 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB23" sqref="AB23"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,13 +892,13 @@
   <sheetData>
     <row r="1" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>15</v>
@@ -910,13 +910,13 @@
         <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>33</v>
@@ -940,43 +940,43 @@
         <v>31</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>0.5</v>
       </c>
       <c r="AC2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
         <v>0.5</v>
       </c>
       <c r="AC3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -1228,25 +1228,25 @@
         <v>1</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -1318,25 +1318,25 @@
         <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -1408,25 +1408,25 @@
         <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
@@ -1498,25 +1498,25 @@
         <v>1</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -1528,7 +1528,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -1588,25 +1588,25 @@
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -1618,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -1678,25 +1678,25 @@
         <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -1708,7 +1708,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
@@ -1723,13 +1723,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I10" s="1">
         <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -1768,25 +1768,25 @@
         <v>1</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -1813,13 +1813,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I11" s="1">
         <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -1858,25 +1858,25 @@
         <v>1</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -1888,7 +1888,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y12" s="1">
         <v>1</v>
@@ -1963,10 +1963,10 @@
         <v>0</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -1993,13 +1993,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I13" s="1">
         <v>8</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
@@ -2038,25 +2038,25 @@
         <v>1</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -2068,7 +2068,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I14" s="1">
         <v>9</v>
@@ -2128,25 +2128,25 @@
         <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC14" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -2158,7 +2158,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -2173,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I15" s="1">
         <v>10</v>
@@ -2218,25 +2218,25 @@
         <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -2248,7 +2248,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I16" s="1">
         <v>11</v>
@@ -2308,25 +2308,25 @@
         <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -2398,25 +2398,25 @@
         <v>1</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -2488,25 +2488,25 @@
         <v>1</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -2518,7 +2518,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -2533,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I19" s="1">
         <v>10</v>
@@ -2587,16 +2587,16 @@
         <v>0</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA19" s="1">
         <v>0</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -2608,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -2623,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I20" s="1">
         <v>10</v>
@@ -2668,25 +2668,25 @@
         <v>1</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -2698,7 +2698,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -2713,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I21" s="1">
         <v>11</v>
@@ -2767,16 +2767,16 @@
         <v>0</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA21" s="1">
         <v>0</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -2788,7 +2788,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -2803,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I22" s="1">
         <v>11</v>
@@ -2848,25 +2848,25 @@
         <v>1</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
@@ -2938,25 +2938,25 @@
         <v>1</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
@@ -3028,25 +3028,25 @@
         <v>1</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC24" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -3058,7 +3058,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -3073,7 +3073,7 @@
         <v>0.9</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1">
         <v>10</v>
@@ -3127,16 +3127,16 @@
         <v>0</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA25" s="1">
         <v>0</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC25" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
@@ -3148,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -3163,7 +3163,7 @@
         <v>0.9</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I26" s="1">
         <v>10</v>
@@ -3208,25 +3208,25 @@
         <v>1</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC26" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
@@ -3238,7 +3238,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -3253,7 +3253,7 @@
         <v>0.9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I27" s="1">
         <v>11</v>
@@ -3307,16 +3307,16 @@
         <v>0</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA27" s="1">
         <v>0</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
@@ -3328,7 +3328,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -3343,7 +3343,7 @@
         <v>0.9</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I28" s="1">
         <v>11</v>
@@ -3388,25 +3388,25 @@
         <v>1</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>